<commit_message>
Pequena revisão no F.Fab. Imagens da placa do atuador e carga. Em edição, novo roteiro para o Projeto Semestral.
</commit_message>
<xml_diff>
--- a/1.3-laboratorio/projetos/z-listas-de-materiais-para-producao-combinadas/2022-projeto-semestral-dg/2022-orcamento-bau-da-eletronica.xlsx
+++ b/1.3-laboratorio/projetos/z-listas-de-materiais-para-producao-combinadas/2022-projeto-semestral-dg/2022-orcamento-bau-da-eletronica.xlsx
@@ -151,6 +151,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -166,12 +167,27 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -179,6 +195,7 @@
       <color rgb="FF1A237E"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -186,12 +203,7 @@
       <color rgb="FF0D47A1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -199,6 +211,7 @@
       <color rgb="FF0D47A1"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -206,21 +219,17 @@
       <color rgb="FF0D47A1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -236,13 +245,7 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7F5E0"/>
-        <bgColor rgb="FFDEEBD7"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFDEEBD7"/>
-        <bgColor rgb="FFE7F5E0"/>
+        <bgColor rgb="FFCCFFCC"/>
       </patternFill>
     </fill>
     <fill>
@@ -285,21 +288,35 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="26">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -308,43 +325,43 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="27" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="27" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="23" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="28" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="28" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="24" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -356,7 +373,7 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -364,15 +381,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,35 +401,19 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -428,15 +429,15 @@
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
-    <cellStyle name="Canto da tabela dinâmica" xfId="20"/>
-    <cellStyle name="Valor da tabela dinâmica" xfId="21"/>
-    <cellStyle name="Campo da tabela dinâmica" xfId="22"/>
-    <cellStyle name="Categoria da tabela dinâmica" xfId="23"/>
-    <cellStyle name="Título da tabela dinâmica" xfId="24"/>
+    <cellStyle name="Campo da tabela dinâmica" xfId="20"/>
+    <cellStyle name="Canto da tabela dinâmica" xfId="21"/>
+    <cellStyle name="Categoria da tabela dinâmica" xfId="22"/>
+    <cellStyle name="Heading 1 1" xfId="23"/>
+    <cellStyle name="Heading 2 2" xfId="24"/>
     <cellStyle name="Resultado da tabela dinâmica" xfId="25"/>
     <cellStyle name="Sem título1" xfId="26"/>
-    <cellStyle name="Heading 1" xfId="27"/>
-    <cellStyle name="Heading 2" xfId="28"/>
+    <cellStyle name="Título da tabela dinâmica" xfId="27"/>
+    <cellStyle name="Valor da tabela dinâmica" xfId="28"/>
   </cellStyles>
   <colors>
     <indexedColors>
@@ -474,7 +475,7 @@
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FF00CCFF"/>
       <rgbColor rgb="FFCCFFFF"/>
-      <rgbColor rgb="FFDEEBD7"/>
+      <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFECB3"/>
       <rgbColor rgb="FF99CCFF"/>
       <rgbColor rgb="FFFF99CC"/>
@@ -512,14 +513,14 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F17" activeCellId="0" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.34"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="23.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="16.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.02"/>
@@ -817,19 +818,19 @@
       <c r="H17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="s">
+      <c r="A18" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="C18" s="23" t="n">
+      <c r="C18" s="19" t="n">
         <v>104</v>
       </c>
-      <c r="D18" s="24" t="n">
+      <c r="D18" s="20" t="n">
         <v>13.9</v>
       </c>
-      <c r="E18" s="25" t="n">
+      <c r="E18" s="21" t="n">
         <f aca="false">C18*D18</f>
         <v>1445.6</v>
       </c>
@@ -840,19 +841,19 @@
       <c r="H18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="s">
+      <c r="A19" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="C19" s="23" t="n">
+      <c r="C19" s="19" t="n">
         <v>19</v>
       </c>
-      <c r="D19" s="24" t="n">
+      <c r="D19" s="20" t="n">
         <v>10</v>
       </c>
-      <c r="E19" s="25" t="n">
+      <c r="E19" s="21" t="n">
         <f aca="false">C19*D19</f>
         <v>190</v>
       </c>
@@ -863,17 +864,17 @@
       <c r="H19" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="15.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="26" t="s">
+      <c r="A21" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="28" t="n">
+      <c r="B21" s="23"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="24" t="n">
         <f aca="false">SUM(E8:E19)</f>
         <v>3440.75</v>
       </c>
-      <c r="F21" s="29"/>
+      <c r="F21" s="25"/>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
     </row>

</xml_diff>